<commit_message>
nowrin AddNew updated and gitignore added
</commit_message>
<xml_diff>
--- a/Nowrin addnew-library.xlsx
+++ b/Nowrin addnew-library.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AKB\Desktop\New folder (4)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D51CBFB0-8948-41C8-AB90-F137039BFA26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8010" yWindow="1350" windowWidth="21600" windowHeight="11385" xr2:uid="{7B6F395A-61F1-42E2-BB0A-89A749CCCC84}"/>
+    <workbookView xWindow="8010" yWindow="1350" windowWidth="21600" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Add New</t>
   </si>
@@ -70,12 +69,24 @@
   </si>
   <si>
     <t>Nowrin</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>10 mins</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>BookTran</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -368,22 +379,10 @@
   </cellStyleXfs>
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -399,6 +398,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -712,11 +723,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C08F9E5D-3BEF-48F9-A10B-403B162DB8AC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:F4"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,97 +741,109 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
     </row>
     <row r="3" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
     </row>
     <row r="4" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
     </row>
     <row r="5" spans="3:10" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="J5" s="2"/>
+      <c r="J5" s="1"/>
     </row>
     <row r="6" spans="3:10" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="J6" s="3"/>
+      <c r="J6" s="2"/>
     </row>
     <row r="7" spans="3:10" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="7"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="3"/>
     </row>
     <row r="8" spans="3:10" ht="22.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="11" t="s">
+      <c r="I8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="7"/>
+      <c r="J8" s="3"/>
     </row>
     <row r="9" spans="3:10" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="21" t="s">
+      <c r="E9" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="13"/>
-      <c r="H9" s="12">
+      <c r="G9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="8">
         <v>2</v>
       </c>
-      <c r="I9" s="20"/>
-      <c r="J9" s="7"/>
+      <c r="I9" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="3"/>
     </row>
     <row r="10" spans="3:10" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="15" t="s">
+      <c r="D10" s="12"/>
+      <c r="E10" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="17"/>
-      <c r="H10" s="16">
+      <c r="G10" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="12">
         <v>3</v>
       </c>
-      <c r="I10" s="18"/>
-      <c r="J10" s="7"/>
+      <c r="I10" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" s="3"/>
     </row>
     <row r="11" spans="3:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>

</xml_diff>